<commit_message>
upload image and notice
</commit_message>
<xml_diff>
--- a/doc/nodejs端接口文档.xlsx
+++ b/doc/nodejs端接口文档.xlsx
@@ -464,7 +464,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>若非员工，插入新数据：???</t>
+    <t xml:space="preserve">插入新数据：UPDATE `db_ars`.`tbl_user` SET `fingerprint`='xxx' WHERE `uid`='1';这个应该是更新吧？先保存好身份证信息，更新头像信息吧！不过现在好像少照片字段
+</t>
+    <rPh sb="0" eb="1">
+      <t>cha'r</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>xin'shu'ju</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">若非员工，插入新数据：INSERT INTO `db_ars`.`tbl_guests` (`created_at`, `uuid`, `image`, `status`) VALUES ( '1521725598', '111111', 'http://xxxx.xxx.xxx/xxxxxxx', '0');
+</t>
     <rPh sb="0" eb="1">
       <t>ruo</t>
     </rPh>
@@ -478,17 +490,6 @@
       <t>cha'r</t>
     </rPh>
     <rPh sb="7" eb="8">
-      <t>xin'shu'ju</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">插入新数据：UPDATE `db_ars`.`tbl_user` SET `fingerprint`='xxx' WHERE `uid`='1';这个应该是更新吧？先保存好身份证信息，更新头像信息吧！不过现在好像少照片字段
-</t>
-    <rPh sb="0" eb="1">
-      <t>cha'r</t>
-    </rPh>
-    <rPh sb="2" eb="3">
       <t>xin'shu'ju</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -714,6 +715,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -722,18 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1019,7 +1020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1030,7 +1031,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1088,10 +1089,10 @@
       <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1111,14 +1112,14 @@
       <c r="J2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="29"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1132,12 +1133,12 @@
         <v>17</v>
       </c>
       <c r="J3" s="26"/>
-      <c r="K3" s="24"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="29"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="8"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1151,12 +1152,12 @@
         <v>18</v>
       </c>
       <c r="J4" s="26"/>
-      <c r="K4" s="24"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="29"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -1170,12 +1171,12 @@
         <v>26</v>
       </c>
       <c r="J5" s="26"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="29"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="10"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -1189,12 +1190,12 @@
         <v>27</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="24"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="29"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1208,12 +1209,12 @@
         <v>28</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="29"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1227,12 +1228,12 @@
         <v>29</v>
       </c>
       <c r="J8" s="26"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="29"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="10"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -1246,12 +1247,12 @@
         <v>30</v>
       </c>
       <c r="J9" s="26"/>
-      <c r="K9" s="24"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="29"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="10"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1265,12 +1266,12 @@
         <v>31</v>
       </c>
       <c r="J10" s="26"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" ht="17" customHeight="1">
       <c r="A11" s="29"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="10"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1284,12 +1285,12 @@
         <v>32</v>
       </c>
       <c r="J11" s="26"/>
-      <c r="K11" s="24"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="29"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="10"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1303,12 +1304,12 @@
         <v>35</v>
       </c>
       <c r="J12" s="27"/>
-      <c r="K12" s="24"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="29"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -1316,12 +1317,12 @@
       <c r="H13" s="7"/>
       <c r="I13" s="17"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="30"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="12"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1329,16 +1330,16 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="26"/>
-      <c r="K14" s="25"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="1:11" ht="26">
-      <c r="A15" s="19">
+      <c r="A15" s="23">
         <v>2</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="23" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1355,17 +1356,17 @@
       <c r="I15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="24" t="s">
+      <c r="K15" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="10"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -1378,13 +1379,13 @@
       <c r="I16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="24"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="10"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1397,43 +1398,43 @@
       <c r="I17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="24"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="10"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="24"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="12"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="25"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="19">
+      <c r="A20" s="23">
         <v>3</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="16" t="s">
@@ -1452,17 +1453,17 @@
         <v>10</v>
       </c>
       <c r="I20" s="13"/>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="23" t="s">
-        <v>51</v>
+      <c r="K20" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1473,13 +1474,13 @@
         <v>16</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="24"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="10"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -1490,43 +1491,43 @@
         <v>14</v>
       </c>
       <c r="I22" s="9"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="24"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="10"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="10"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="24"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="12"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="12"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="25"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="19">
+      <c r="A25" s="23">
         <v>4</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="16" t="s">
@@ -1545,17 +1546,17 @@
         <v>10</v>
       </c>
       <c r="I25" s="13"/>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K25" s="23" t="s">
-        <v>52</v>
+      <c r="K25" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="10" t="s">
         <v>34</v>
       </c>
@@ -1572,13 +1573,13 @@
         <v>16</v>
       </c>
       <c r="I26" s="9"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="24"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="10"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1589,37 +1590,42 @@
         <v>14</v>
       </c>
       <c r="I27" s="9"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="24"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="10"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="24"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="21"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="12"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="25"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="J25:J29"/>
+    <mergeCell ref="K25:K29"/>
     <mergeCell ref="J15:J19"/>
     <mergeCell ref="K2:K14"/>
     <mergeCell ref="K15:K19"/>
@@ -1635,11 +1641,6 @@
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="B2:B14"/>
     <mergeCell ref="C2:C14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="J25:J29"/>
-    <mergeCell ref="K25:K29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>